<commit_message>
Added negative test cases for Header module
</commit_message>
<xml_diff>
--- a/Excel/Book2.xlsx
+++ b/Excel/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New\school-automation\Erp_school\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2157FE58-D84B-44EA-83C3-0E4D8F08EFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EAA49E-5BE5-467F-A167-1A1B1ABF3A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C65AA738-EF8D-47CE-9D2F-830EF9A9F920}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Test_id</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Driver</t>
+  </si>
+  <si>
+    <t>Prasannaee</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD9148B-8DA4-4EBA-92A4-0C6C516CA800}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C4" sqref="C4:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,6 +606,50 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>900</v>
+      </c>
+      <c r="H4" s="1">
+        <v>35822</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>9876543210</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="1">
+        <v>45563</v>
+      </c>
+      <c r="N4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4">
+        <v>654329</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" xr:uid="{ADD22963-206D-4F50-A51C-A5C18FC2A61F}"/>

</xml_diff>